<commit_message>
NIH kjørt stiff, lagt div i grphpad
</commit_message>
<xml_diff>
--- a/data_output/output for F24 stiff 2018-01-18 youngs modulus/all_stiff_output_20180118_1237 GM.xlsx
+++ b/data_output/output for F24 stiff 2018-01-18 youngs modulus/all_stiff_output_20180118_1237 GM.xlsx
@@ -153,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,13 +161,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -179,15 +191,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Nøytral" xfId="1" builtinId="28"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -467,11 +483,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="16" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="20" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="5.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="31" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="32" max="35" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -522,7 +546,7 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="R1" t="s">
@@ -534,7 +558,7 @@
       <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="2" t="s">
         <v>20</v>
       </c>
       <c r="V1" t="s">
@@ -632,7 +656,7 @@
       <c r="P2">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="2">
         <v>324.81294026305056</v>
       </c>
       <c r="R2">
@@ -644,7 +668,7 @@
       <c r="T2">
         <v>264.41477666127167</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="2">
         <v>269.79820525079003</v>
       </c>
       <c r="V2">
@@ -742,7 +766,7 @@
       <c r="P3">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="2">
         <v>358.23379352322382</v>
       </c>
       <c r="R3">
@@ -754,7 +778,7 @@
       <c r="T3">
         <v>271.76478876458299</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="2">
         <v>279.66003195314016</v>
       </c>
       <c r="V3">
@@ -852,7 +876,7 @@
       <c r="P4">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="2">
         <v>265.22123940810724</v>
       </c>
       <c r="R4">
@@ -864,7 +888,7 @@
       <c r="T4">
         <v>251.64497340760192</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="2">
         <v>252.79040230269538</v>
       </c>
       <c r="V4">
@@ -962,7 +986,7 @@
       <c r="P5">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="2">
         <v>303.00386139964723</v>
       </c>
       <c r="R5">
@@ -974,7 +998,7 @@
       <c r="T5">
         <v>268.35060640205097</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="2">
         <v>271.34855050652635</v>
       </c>
       <c r="V5">
@@ -1072,7 +1096,7 @@
       <c r="P6">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="2">
         <v>432.77188335382021</v>
       </c>
       <c r="R6">
@@ -1084,7 +1108,7 @@
       <c r="T6">
         <v>403.07910975531246</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="2">
         <v>414.93508957150414</v>
       </c>
       <c r="V6">
@@ -1182,7 +1206,7 @@
       <c r="P7">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="2">
         <v>406.17728511702006</v>
       </c>
       <c r="R7">
@@ -1194,7 +1218,7 @@
       <c r="T7">
         <v>379.0418949203339</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="2">
         <v>389.87797082247488</v>
       </c>
       <c r="V7">
@@ -1292,7 +1316,7 @@
       <c r="P8">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="2">
         <v>393.03027214478919</v>
       </c>
       <c r="R8">
@@ -1304,7 +1328,7 @@
       <c r="T8">
         <v>361.90993089440502</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="2">
         <v>372.59891768961506</v>
       </c>
       <c r="V8">
@@ -1402,7 +1426,7 @@
       <c r="P9">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="2">
         <v>356.51403260698112</v>
       </c>
       <c r="R9">
@@ -1414,7 +1438,7 @@
       <c r="T9">
         <v>329.54052493153671</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="2">
         <v>338.80559738624527</v>
       </c>
       <c r="V9">
@@ -1512,7 +1536,7 @@
       <c r="P10">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="2">
         <v>336.13164874081986</v>
       </c>
       <c r="R10">
@@ -1524,7 +1548,7 @@
       <c r="T10">
         <v>276.53641756063769</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="2">
         <v>283.44709309240392</v>
       </c>
       <c r="V10">
@@ -1622,7 +1646,7 @@
       <c r="P11">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="2">
         <v>303.6591217788029</v>
       </c>
       <c r="R11">
@@ -1634,7 +1658,7 @@
       <c r="T11">
         <v>246.85896372988208</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="2">
         <v>253.46835552615909</v>
       </c>
       <c r="V11">
@@ -1732,7 +1756,7 @@
       <c r="P12">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="2">
         <v>264.97236445464893</v>
       </c>
       <c r="R12">
@@ -1744,7 +1768,7 @@
       <c r="T12">
         <v>214.00387946975329</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="2">
         <v>219.4702257675126</v>
       </c>
       <c r="V12">
@@ -1842,7 +1866,7 @@
       <c r="P13">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q13">
+      <c r="Q13" s="2">
         <v>264.68029527884056</v>
       </c>
       <c r="R13">
@@ -1854,7 +1878,7 @@
       <c r="T13">
         <v>214.94587294427745</v>
       </c>
-      <c r="U13">
+      <c r="U13" s="2">
         <v>220.27085376863405</v>
       </c>
       <c r="V13">
@@ -1952,7 +1976,7 @@
       <c r="P14">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q14">
+      <c r="Q14" s="2">
         <v>444.13542968101621</v>
       </c>
       <c r="R14">
@@ -1964,7 +1988,7 @@
       <c r="T14">
         <v>450.63116470149788</v>
       </c>
-      <c r="U14">
+      <c r="U14" s="2">
         <v>464.06762423232578</v>
       </c>
       <c r="V14">
@@ -2062,7 +2086,7 @@
       <c r="P15">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q15">
+      <c r="Q15" s="2">
         <v>265.6447730749066</v>
       </c>
       <c r="R15">
@@ -2074,7 +2098,7 @@
       <c r="T15">
         <v>269.22755311872669</v>
       </c>
-      <c r="U15">
+      <c r="U15" s="2">
         <v>276.71561372920115</v>
       </c>
       <c r="V15">
@@ -2172,7 +2196,7 @@
       <c r="P16">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q16">
+      <c r="Q16" s="2">
         <v>366.67806811889511</v>
       </c>
       <c r="R16">
@@ -2184,7 +2208,7 @@
       <c r="T16">
         <v>349.29348177089219</v>
       </c>
-      <c r="U16">
+      <c r="U16" s="2">
         <v>359.66182738846618</v>
       </c>
       <c r="V16">
@@ -2282,7 +2306,7 @@
       <c r="P17">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q17">
+      <c r="Q17" s="2">
         <v>348.20994402053839</v>
       </c>
       <c r="R17">
@@ -2294,7 +2318,7 @@
       <c r="T17">
         <v>332.34544595222468</v>
       </c>
-      <c r="U17">
+      <c r="U17" s="2">
         <v>341.80999221379551</v>
       </c>
       <c r="V17">
@@ -2392,7 +2416,7 @@
       <c r="P18">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="2">
         <v>307.8046746090078</v>
       </c>
       <c r="R18">
@@ -2404,7 +2428,7 @@
       <c r="T18">
         <v>260.69729734569904</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="2">
         <v>265.30267887957757</v>
       </c>
       <c r="V18">
@@ -2502,7 +2526,7 @@
       <c r="P19">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q19">
+      <c r="Q19" s="2">
         <v>328.05410430190886</v>
       </c>
       <c r="R19">
@@ -2514,7 +2538,7 @@
       <c r="T19">
         <v>265.53456216733809</v>
       </c>
-      <c r="U19">
+      <c r="U19" s="2">
         <v>271.73859443070427</v>
       </c>
       <c r="V19">
@@ -2612,7 +2636,7 @@
       <c r="P20">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q20">
+      <c r="Q20" s="2">
         <v>275.37127714804262</v>
       </c>
       <c r="R20">
@@ -2624,7 +2648,7 @@
       <c r="T20">
         <v>255.78740504243666</v>
       </c>
-      <c r="U20">
+      <c r="U20" s="2">
         <v>257.29792953322396</v>
       </c>
       <c r="V20">
@@ -2722,7 +2746,7 @@
       <c r="P21">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q21">
+      <c r="Q21" s="2">
         <v>356.72305557959493</v>
       </c>
       <c r="R21">
@@ -2734,7 +2758,7 @@
       <c r="T21">
         <v>273.39600032171546</v>
       </c>
-      <c r="U21">
+      <c r="U21" s="2">
         <v>280.2962733309044</v>
       </c>
       <c r="V21">
@@ -2832,7 +2856,7 @@
       <c r="P22">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q22">
+      <c r="Q22" s="2">
         <v>424.1633417530465</v>
       </c>
       <c r="R22">
@@ -2844,7 +2868,7 @@
       <c r="T22">
         <v>357.0271869623395</v>
       </c>
-      <c r="U22">
+      <c r="U22" s="2">
         <v>366.41089917850087</v>
       </c>
       <c r="V22">
@@ -2942,7 +2966,7 @@
       <c r="P23">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q23">
+      <c r="Q23" s="2">
         <v>366.82632259704968</v>
       </c>
       <c r="R23">
@@ -2954,7 +2978,7 @@
       <c r="T23">
         <v>305.819951841229</v>
       </c>
-      <c r="U23">
+      <c r="U23" s="2">
         <v>314.36709916636448</v>
       </c>
       <c r="V23">
@@ -3052,7 +3076,7 @@
       <c r="P24">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q24">
+      <c r="Q24" s="2">
         <v>340.50833562903154</v>
       </c>
       <c r="R24">
@@ -3064,7 +3088,7 @@
       <c r="T24">
         <v>300.47482586426855</v>
       </c>
-      <c r="U24">
+      <c r="U24" s="2">
         <v>307.07421105613713</v>
       </c>
       <c r="V24">
@@ -3162,7 +3186,7 @@
       <c r="P25">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q25">
+      <c r="Q25" s="2">
         <v>329.56856075439413</v>
       </c>
       <c r="R25">
@@ -3174,7 +3198,7 @@
       <c r="T25">
         <v>281.91685812666316</v>
       </c>
-      <c r="U25">
+      <c r="U25" s="2">
         <v>289.82351095126791</v>
       </c>
       <c r="V25">
@@ -3272,7 +3296,7 @@
       <c r="P26">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q26">
+      <c r="Q26" s="2">
         <v>441.11773417630013</v>
       </c>
       <c r="R26">
@@ -3284,7 +3308,7 @@
       <c r="T26">
         <v>331.14335442351683</v>
       </c>
-      <c r="U26">
+      <c r="U26" s="2">
         <v>338.73264978534576</v>
       </c>
       <c r="V26">
@@ -3382,7 +3406,7 @@
       <c r="P27">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q27">
+      <c r="Q27" s="2">
         <v>401.1138651270573</v>
       </c>
       <c r="R27">
@@ -3394,7 +3418,7 @@
       <c r="T27">
         <v>286.99160812469273</v>
       </c>
-      <c r="U27">
+      <c r="U27" s="2">
         <v>295.01520900778547</v>
       </c>
       <c r="V27">
@@ -3492,7 +3516,7 @@
       <c r="P28">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q28">
+      <c r="Q28" s="2">
         <v>428.2870739294741</v>
       </c>
       <c r="R28">
@@ -3504,7 +3528,7 @@
       <c r="T28">
         <v>310.41588348590716</v>
       </c>
-      <c r="U28">
+      <c r="U28" s="2">
         <v>318.66188537197968</v>
       </c>
       <c r="V28">
@@ -3602,7 +3626,7 @@
       <c r="P29">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q29">
+      <c r="Q29" s="2">
         <v>440.81451406213068</v>
       </c>
       <c r="R29">
@@ -3614,7 +3638,7 @@
       <c r="T29">
         <v>312.52417226736827</v>
       </c>
-      <c r="U29">
+      <c r="U29" s="2">
         <v>321.57567256326234</v>
       </c>
       <c r="V29">
@@ -3712,7 +3736,7 @@
       <c r="P30">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q30">
+      <c r="Q30" s="2">
         <v>297.89499185830971</v>
       </c>
       <c r="R30">
@@ -3724,7 +3748,7 @@
       <c r="T30">
         <v>255.66763839883126</v>
       </c>
-      <c r="U30">
+      <c r="U30" s="2">
         <v>263.14924743727858</v>
       </c>
       <c r="V30">
@@ -3822,7 +3846,7 @@
       <c r="P31">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q31">
+      <c r="Q31" s="2">
         <v>311.05820708003375</v>
       </c>
       <c r="R31">
@@ -3834,7 +3858,7 @@
       <c r="T31">
         <v>271.23820793723075</v>
       </c>
-      <c r="U31">
+      <c r="U31" s="2">
         <v>278.27226884594455</v>
       </c>
       <c r="V31">
@@ -3932,7 +3956,7 @@
       <c r="P32">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q32">
+      <c r="Q32" s="2">
         <v>277.09130476851783</v>
       </c>
       <c r="R32">
@@ -3944,7 +3968,7 @@
       <c r="T32">
         <v>243.20137214901257</v>
       </c>
-      <c r="U32">
+      <c r="U32" s="2">
         <v>250.13878789208374</v>
       </c>
       <c r="V32">
@@ -4042,7 +4066,7 @@
       <c r="P33">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q33">
+      <c r="Q33" s="2">
         <v>282.39790219946445</v>
       </c>
       <c r="R33">
@@ -4054,7 +4078,7 @@
       <c r="T33">
         <v>249.10460798444402</v>
       </c>
-      <c r="U33">
+      <c r="U33" s="2">
         <v>255.91484068796234</v>
       </c>
       <c r="V33">
@@ -4152,7 +4176,7 @@
       <c r="P34">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q34">
+      <c r="Q34" s="2">
         <v>360.72864033149028</v>
       </c>
       <c r="R34">
@@ -4164,7 +4188,7 @@
       <c r="T34">
         <v>309.52243122698786</v>
       </c>
-      <c r="U34">
+      <c r="U34" s="2">
         <v>318.01352844055344</v>
       </c>
       <c r="V34">
@@ -4262,7 +4286,7 @@
       <c r="P35">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q35">
+      <c r="Q35" s="2">
         <v>393.19280105867068</v>
       </c>
       <c r="R35">
@@ -4274,7 +4298,7 @@
       <c r="T35">
         <v>335.52748493947871</v>
       </c>
-      <c r="U35">
+      <c r="U35" s="2">
         <v>345.10037124487621</v>
       </c>
       <c r="V35">
@@ -4372,7 +4396,7 @@
       <c r="P36">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q36">
+      <c r="Q36" s="2">
         <v>352.44920446115162</v>
       </c>
       <c r="R36">
@@ -4384,7 +4408,7 @@
       <c r="T36">
         <v>295.41335820038995</v>
       </c>
-      <c r="U36">
+      <c r="U36" s="2">
         <v>303.84350436788628</v>
       </c>
       <c r="V36">
@@ -4482,7 +4506,7 @@
       <c r="P37">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q37">
+      <c r="Q37" s="2">
         <v>440.84079940992535</v>
       </c>
       <c r="R37">
@@ -4494,7 +4518,7 @@
       <c r="T37">
         <v>366.91090407173243</v>
       </c>
-      <c r="U37">
+      <c r="U37" s="2">
         <v>377.85579165035267</v>
       </c>
       <c r="V37">
@@ -4592,7 +4616,7 @@
       <c r="P38">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q38">
+      <c r="Q38" s="2">
         <v>270.06476839245698</v>
       </c>
       <c r="R38">
@@ -4604,7 +4628,7 @@
       <c r="T38">
         <v>231.71251904646792</v>
       </c>
-      <c r="U38">
+      <c r="U38" s="2">
         <v>236.53025105155393</v>
       </c>
       <c r="V38">
@@ -4702,7 +4726,7 @@
       <c r="P39">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q39">
+      <c r="Q39" s="2">
         <v>369.43529467746049</v>
       </c>
       <c r="R39">
@@ -4714,7 +4738,7 @@
       <c r="T39">
         <v>301.07722171172105</v>
       </c>
-      <c r="U39">
+      <c r="U39" s="2">
         <v>309.7857248030507</v>
       </c>
       <c r="V39">
@@ -4812,7 +4836,7 @@
       <c r="P40">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q40">
+      <c r="Q40" s="2">
         <v>311.23708130039097</v>
       </c>
       <c r="R40">
@@ -4824,7 +4848,7 @@
       <c r="T40">
         <v>265.84592272664219</v>
       </c>
-      <c r="U40">
+      <c r="U40" s="2">
         <v>272.9266724582078</v>
       </c>
       <c r="V40">
@@ -4922,7 +4946,7 @@
       <c r="P41">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q41">
+      <c r="Q41" s="2">
         <v>326.7122099622415</v>
       </c>
       <c r="R41">
@@ -4934,7 +4958,7 @@
       <c r="T41">
         <v>276.57432174186755</v>
       </c>
-      <c r="U41">
+      <c r="U41" s="2">
         <v>284.41096511975553</v>
       </c>
       <c r="V41">
@@ -4983,443 +5007,443 @@
         <v>0.89132999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A42">
+    <row r="42" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="2">
         <v>13</v>
       </c>
-      <c r="B42" t="s">
+      <c r="B42" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D42" t="s">
+      <c r="D42" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="2">
         <v>5.5166681099999997E-2</v>
       </c>
-      <c r="F42">
-        <v>0</v>
-      </c>
-      <c r="G42">
+      <c r="F42" s="2">
+        <v>0</v>
+      </c>
+      <c r="G42" s="2">
         <v>26.300787106331217</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="2">
         <v>101.55936578098198</v>
       </c>
-      <c r="I42">
-        <v>0</v>
-      </c>
-      <c r="J42">
+      <c r="I42" s="2">
+        <v>0</v>
+      </c>
+      <c r="J42" s="2">
         <v>0.98667398163886255</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="2">
         <v>2550</v>
       </c>
-      <c r="L42">
+      <c r="L42" s="2">
         <v>4474.2342157431194</v>
       </c>
-      <c r="M42">
+      <c r="M42" s="2">
         <v>4450</v>
       </c>
-      <c r="N42">
+      <c r="N42" s="2">
         <v>5038.7556635617384</v>
       </c>
-      <c r="O42">
+      <c r="O42" s="2">
         <v>1800</v>
       </c>
-      <c r="P42">
+      <c r="P42" s="2">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q42">
+      <c r="Q42" s="2">
         <v>501.03775424705105</v>
       </c>
-      <c r="R42">
+      <c r="R42" s="2">
         <v>514.78072623105072</v>
       </c>
-      <c r="S42">
+      <c r="S42" s="2">
         <v>424.55392879818373</v>
       </c>
-      <c r="T42">
+      <c r="T42" s="2">
         <v>435.99746372637236</v>
       </c>
-      <c r="U42">
+      <c r="U42" s="2">
         <v>448.34118111193499</v>
       </c>
-      <c r="V42">
+      <c r="V42" s="2">
         <v>460.50382940036059</v>
       </c>
-      <c r="W42">
+      <c r="W42" s="2">
         <v>7.6553547630905747</v>
       </c>
-      <c r="X42">
+      <c r="X42" s="2">
         <v>10.08400141357524</v>
       </c>
-      <c r="Y42">
+      <c r="Y42" s="2">
         <v>6.7343988079329229</v>
       </c>
-      <c r="Z42">
+      <c r="Z42" s="2">
         <v>7.18055678981254</v>
       </c>
-      <c r="AA42">
+      <c r="AA42" s="2">
         <v>177.296666666666</v>
       </c>
-      <c r="AB42">
+      <c r="AB42" s="2">
         <v>4.3178221604602101</v>
       </c>
-      <c r="AC42">
+      <c r="AC42" s="2">
         <v>5.6876429789478715</v>
       </c>
-      <c r="AD42">
+      <c r="AD42" s="2">
         <v>3.7983786917969589</v>
       </c>
-      <c r="AE42">
+      <c r="AE42" s="2">
         <v>4.0500235705573902</v>
       </c>
-      <c r="AF42" s="1">
+      <c r="AF42" s="3">
         <v>3325510838.0548935</v>
       </c>
-      <c r="AG42" s="1">
+      <c r="AG42" s="3">
         <v>1363656761.0737436</v>
       </c>
-      <c r="AH42" s="1">
+      <c r="AH42" s="3">
         <v>1668796685.7065408</v>
       </c>
-      <c r="AI42" s="1">
+      <c r="AI42" s="3">
         <v>1854424906.3169391</v>
       </c>
-      <c r="AJ42">
+      <c r="AJ42" s="2">
         <v>0.56144000000000005</v>
       </c>
     </row>
-    <row r="43" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A43">
+    <row r="43" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2">
         <v>13</v>
       </c>
-      <c r="B43" t="s">
+      <c r="B43" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D43" t="s">
+      <c r="D43" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="2">
         <v>5.5166681099999997E-2</v>
       </c>
-      <c r="F43">
-        <v>0</v>
-      </c>
-      <c r="G43">
+      <c r="F43" s="2">
+        <v>0</v>
+      </c>
+      <c r="G43" s="2">
         <v>15.544176624904127</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="2">
         <v>103.81198262293482</v>
       </c>
-      <c r="I43">
-        <v>0</v>
-      </c>
-      <c r="J43">
+      <c r="I43" s="2">
+        <v>0</v>
+      </c>
+      <c r="J43" s="2">
         <v>0.99352542675688316</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="2">
         <v>2550</v>
       </c>
-      <c r="L43">
+      <c r="L43" s="2">
         <v>4766.0784333758347</v>
       </c>
-      <c r="M43">
+      <c r="M43" s="2">
         <v>4750</v>
       </c>
-      <c r="N43">
+      <c r="N43" s="2">
         <v>4700.1725550070196</v>
       </c>
-      <c r="O43">
+      <c r="O43" s="2">
         <v>1800</v>
       </c>
-      <c r="P43">
+      <c r="P43" s="2">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q43">
+      <c r="Q43" s="2">
         <v>391.23123441853107</v>
       </c>
-      <c r="R43">
+      <c r="R43" s="2">
         <v>401.62494414171385</v>
       </c>
-      <c r="S43">
+      <c r="S43" s="2">
         <v>333.4990931290551</v>
       </c>
-      <c r="T43">
+      <c r="T43" s="2">
         <v>342.09969849913972</v>
       </c>
-      <c r="U43">
+      <c r="U43" s="2">
         <v>351.41652455203445</v>
       </c>
-      <c r="V43">
+      <c r="V43" s="2">
         <v>360.57850139573389</v>
       </c>
-      <c r="W43">
+      <c r="W43" s="2">
         <v>9.4597435714104279</v>
       </c>
-      <c r="X43">
+      <c r="X43" s="2">
         <v>11.67542034295594</v>
       </c>
-      <c r="Y43">
+      <c r="Y43" s="2">
         <v>8.1648973320770679</v>
       </c>
-      <c r="Z43">
+      <c r="Z43" s="2">
         <v>8.7166059511648051</v>
       </c>
-      <c r="AA43">
+      <c r="AA43" s="2">
         <v>171.14666666666599</v>
       </c>
-      <c r="AB43">
+      <c r="AB43" s="2">
         <v>5.5272730434386483</v>
       </c>
-      <c r="AC43">
+      <c r="AC43" s="2">
         <v>6.8218800695052897</v>
       </c>
-      <c r="AD43">
+      <c r="AD43" s="2">
         <v>4.7707019313320549</v>
       </c>
-      <c r="AE43">
+      <c r="AE43" s="2">
         <v>5.0930620624599792</v>
       </c>
-      <c r="AF43" s="1">
+      <c r="AF43" s="3">
         <v>1579341863.0414453</v>
       </c>
-      <c r="AG43" s="1">
+      <c r="AG43" s="3">
         <v>1576666993.4982579</v>
       </c>
-      <c r="AH43" s="1">
+      <c r="AH43" s="3">
         <v>765108519.13281941</v>
       </c>
-      <c r="AI43" s="1">
+      <c r="AI43" s="3">
         <v>1018831374.1938319</v>
       </c>
-      <c r="AJ43">
+      <c r="AJ43" s="2">
         <v>0.72911000000000004</v>
       </c>
     </row>
-    <row r="44" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A44">
+    <row r="44" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="2">
         <v>13</v>
       </c>
-      <c r="B44" t="s">
+      <c r="B44" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D44" t="s">
+      <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="2">
         <v>5.46177589E-2</v>
       </c>
-      <c r="F44">
-        <v>0</v>
-      </c>
-      <c r="G44">
+      <c r="F44" s="2">
+        <v>0</v>
+      </c>
+      <c r="G44" s="2">
         <v>55.301972146614368</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="2">
         <v>-22.513744116510217</v>
       </c>
-      <c r="I44">
-        <v>0</v>
-      </c>
-      <c r="J44">
+      <c r="I44" s="2">
+        <v>0</v>
+      </c>
+      <c r="J44" s="2">
         <v>0.98160438617895507</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="2">
         <v>2800</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="2">
         <v>3268.2338192959114</v>
       </c>
-      <c r="M44">
+      <c r="M44" s="2">
         <v>3250</v>
       </c>
-      <c r="N44">
+      <c r="N44" s="2">
         <v>3260.1887792861489</v>
       </c>
-      <c r="O44">
+      <c r="O44" s="2">
         <v>1800</v>
       </c>
-      <c r="P44">
+      <c r="P44" s="2">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q44">
+      <c r="Q44" s="2">
         <v>745.80592413319403</v>
       </c>
-      <c r="R44">
+      <c r="R44" s="2">
         <v>767.14563999111692</v>
       </c>
-      <c r="S44">
+      <c r="S44" s="2">
         <v>598.12686831250221</v>
       </c>
-      <c r="T44">
+      <c r="T44" s="2">
         <v>615.23212778674667</v>
       </c>
-      <c r="U44">
+      <c r="U44" s="2">
         <v>633.57303800711622</v>
       </c>
-      <c r="V44">
+      <c r="V44" s="2">
         <v>651.69486913161472</v>
       </c>
-      <c r="W44">
+      <c r="W44" s="2">
         <v>7.0335781611098849</v>
       </c>
-      <c r="X44">
+      <c r="X44" s="2">
         <v>7.1036061005186024</v>
       </c>
-      <c r="Y44">
+      <c r="Y44" s="2">
         <v>5.9119290665433031</v>
       </c>
-      <c r="Z44">
+      <c r="Z44" s="2">
         <v>6.310579241062154</v>
       </c>
-      <c r="AA44">
+      <c r="AA44" s="2">
         <v>180.22333333333299</v>
       </c>
-      <c r="AB44">
+      <c r="AB44" s="2">
         <v>3.9027011824827889</v>
       </c>
-      <c r="AC44">
+      <c r="AC44" s="2">
         <v>3.9415573827946524</v>
       </c>
-      <c r="AD44">
+      <c r="AD44" s="2">
         <v>3.2803349917010269</v>
       </c>
-      <c r="AE44">
+      <c r="AE44" s="2">
         <v>3.5015328616691321</v>
       </c>
-      <c r="AF44" s="1">
+      <c r="AF44" s="3">
         <v>3492188615.9695535</v>
       </c>
-      <c r="AG44" s="1">
+      <c r="AG44" s="3">
         <v>11840321774.723803</v>
       </c>
-      <c r="AH44" s="1">
+      <c r="AH44" s="3">
         <v>3931226680.2366195</v>
       </c>
-      <c r="AI44" s="1">
+      <c r="AI44" s="3">
         <v>2330526374.7299404</v>
       </c>
-      <c r="AJ44">
+      <c r="AJ44" s="2">
         <v>0.62156</v>
       </c>
     </row>
-    <row r="45" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A45">
+    <row r="45" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="2">
         <v>13</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B45" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D45" t="s">
+      <c r="D45" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="2">
         <v>5.46177589E-2</v>
       </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-      <c r="G45">
+      <c r="F45" s="2">
+        <v>0</v>
+      </c>
+      <c r="G45" s="2">
         <v>27.205941597018843</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="2">
         <v>67.380990431369014</v>
       </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
+      <c r="I45" s="2">
+        <v>0</v>
+      </c>
+      <c r="J45" s="2">
         <v>0.98012150532939257</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="2">
         <v>2800</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="2">
         <v>4395.9803281598797</v>
       </c>
-      <c r="M45">
+      <c r="M45" s="2">
         <v>4350</v>
       </c>
-      <c r="N45">
+      <c r="N45" s="2">
         <v>4668.5808162165749</v>
       </c>
-      <c r="O45">
+      <c r="O45" s="2">
         <v>1800</v>
       </c>
-      <c r="P45">
+      <c r="P45" s="2">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q45">
+      <c r="Q45" s="2">
         <v>527.20106702416308</v>
       </c>
-      <c r="R45">
+      <c r="R45" s="2">
         <v>542.04604471151822</v>
       </c>
-      <c r="S45">
+      <c r="S45" s="2">
         <v>424.62062654803316</v>
       </c>
-      <c r="T45">
+      <c r="T45" s="2">
         <v>436.46644122188394</v>
       </c>
-      <c r="U45">
+      <c r="U45" s="2">
         <v>449.20027697158406</v>
       </c>
-      <c r="V45">
+      <c r="V45" s="2">
         <v>461.7672759124776</v>
       </c>
-      <c r="W45">
+      <c r="W45" s="2">
         <v>8.3668499068530036</v>
       </c>
-      <c r="X45">
+      <c r="X45" s="2">
         <v>10.115218809206963</v>
       </c>
-      <c r="Y45">
+      <c r="Y45" s="2">
         <v>7.3687338066146113</v>
       </c>
-      <c r="Z45">
+      <c r="Z45" s="2">
         <v>7.8150768015337748</v>
       </c>
-      <c r="AA45">
+      <c r="AA45" s="2">
         <v>170.97333333333299</v>
       </c>
-      <c r="AB45">
+      <c r="AB45" s="2">
         <v>4.8936578258907941</v>
       </c>
-      <c r="AC45">
+      <c r="AC45" s="2">
         <v>5.9162552498676115</v>
       </c>
-      <c r="AD45">
+      <c r="AD45" s="2">
         <v>4.3098731614762293</v>
       </c>
-      <c r="AE45">
+      <c r="AE45" s="2">
         <v>4.5709331678627025</v>
       </c>
-      <c r="AF45" s="1">
+      <c r="AF45" s="3">
         <v>3617714038.2978764</v>
       </c>
-      <c r="AG45" s="1">
+      <c r="AG45" s="3">
         <v>1740693358.001543</v>
       </c>
-      <c r="AH45" s="1">
+      <c r="AH45" s="3">
         <v>1055701478.512863</v>
       </c>
-      <c r="AI45" s="1">
+      <c r="AI45" s="3">
         <v>1314668097.0567031</v>
       </c>
-      <c r="AJ45">
+      <c r="AJ45" s="2">
         <v>0.58667000000000002</v>
       </c>
     </row>
@@ -5472,7 +5496,7 @@
       <c r="P46">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q46">
+      <c r="Q46" s="2">
         <v>376.7925723880175</v>
       </c>
       <c r="R46">
@@ -5484,7 +5508,7 @@
       <c r="T46">
         <v>272.2377836895846</v>
       </c>
-      <c r="U46">
+      <c r="U46" s="2">
         <v>280.35697178037532</v>
       </c>
       <c r="V46">
@@ -5582,7 +5606,7 @@
       <c r="P47">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q47">
+      <c r="Q47" s="2">
         <v>331.5729336984441</v>
       </c>
       <c r="R47">
@@ -5594,7 +5618,7 @@
       <c r="T47">
         <v>244.89861623000513</v>
       </c>
-      <c r="U47">
+      <c r="U47" s="2">
         <v>251.57506383108165</v>
       </c>
       <c r="V47">
@@ -5692,7 +5716,7 @@
       <c r="P48">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q48">
+      <c r="Q48" s="2">
         <v>439.31224059849467</v>
       </c>
       <c r="R48">
@@ -5704,7 +5728,7 @@
       <c r="T48">
         <v>307.37902748960164</v>
       </c>
-      <c r="U48">
+      <c r="U48" s="2">
         <v>316.51229893776127</v>
       </c>
       <c r="V48">
@@ -5802,7 +5826,7 @@
       <c r="P49">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q49">
+      <c r="Q49" s="2">
         <v>541.07189803289521</v>
       </c>
       <c r="R49">
@@ -5814,7 +5838,7 @@
       <c r="T49">
         <v>378.36394111525351</v>
       </c>
-      <c r="U49">
+      <c r="U49" s="2">
         <v>389.63010961669278</v>
       </c>
       <c r="V49">
@@ -5912,7 +5936,7 @@
       <c r="P50">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q50">
+      <c r="Q50" s="2">
         <v>236.24489865364842</v>
       </c>
       <c r="R50">
@@ -5924,7 +5948,7 @@
       <c r="T50">
         <v>230.80388865619395</v>
       </c>
-      <c r="U50">
+      <c r="U50" s="2">
         <v>237.36553847472302</v>
       </c>
       <c r="V50">
@@ -6022,7 +6046,7 @@
       <c r="P51">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q51">
+      <c r="Q51" s="2">
         <v>219.43481028834731</v>
       </c>
       <c r="R51">
@@ -6034,7 +6058,7 @@
       <c r="T51">
         <v>214.65831008400673</v>
       </c>
-      <c r="U51">
+      <c r="U51" s="2">
         <v>220.41668459084858</v>
       </c>
       <c r="V51">
@@ -6132,7 +6156,7 @@
       <c r="P52">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q52">
+      <c r="Q52" s="2">
         <v>233.13581365411918</v>
       </c>
       <c r="R52">
@@ -6144,7 +6168,7 @@
       <c r="T52">
         <v>239.18595950442281</v>
       </c>
-      <c r="U52">
+      <c r="U52" s="2">
         <v>245.73603334512208</v>
       </c>
       <c r="V52">
@@ -6234,7 +6258,7 @@
       <c r="P53">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q53">
+      <c r="Q53" s="2">
         <v>190.36134811101167</v>
       </c>
       <c r="R53">
@@ -6246,7 +6270,7 @@
       <c r="T53">
         <v>195.2923626286383</v>
       </c>
-      <c r="U53">
+      <c r="U53" s="2">
         <v>200.63176571799414</v>
       </c>
       <c r="V53">
@@ -6344,7 +6368,7 @@
       <c r="P54">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q54">
+      <c r="Q54" s="2">
         <v>367.49097405477858</v>
       </c>
       <c r="R54">
@@ -6356,7 +6380,7 @@
       <c r="T54">
         <v>275.04866833252697</v>
       </c>
-      <c r="U54">
+      <c r="U54" s="2">
         <v>279.19013686541996</v>
       </c>
       <c r="V54">
@@ -6454,7 +6478,7 @@
       <c r="P55">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q55">
+      <c r="Q55" s="2">
         <v>386.59125695824753</v>
       </c>
       <c r="R55">
@@ -6466,7 +6490,7 @@
       <c r="T55">
         <v>268.30520449453411</v>
       </c>
-      <c r="U55">
+      <c r="U55" s="2">
         <v>273.78880987200029</v>
       </c>
       <c r="V55">
@@ -6564,7 +6588,7 @@
       <c r="P56">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q56">
+      <c r="Q56" s="2">
         <v>469.15858224360278</v>
       </c>
       <c r="R56">
@@ -6576,7 +6600,7 @@
       <c r="T56">
         <v>327.02160292627235</v>
       </c>
-      <c r="U56">
+      <c r="U56" s="2">
         <v>334.41773710028178</v>
       </c>
       <c r="V56">
@@ -6674,7 +6698,7 @@
       <c r="P57">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q57">
+      <c r="Q57" s="2">
         <v>431.19933117129182</v>
       </c>
       <c r="R57">
@@ -6686,7 +6710,7 @@
       <c r="T57">
         <v>323.57378496004281</v>
       </c>
-      <c r="U57">
+      <c r="U57" s="2">
         <v>328.99635827316752</v>
       </c>
       <c r="V57">
@@ -6784,7 +6808,7 @@
       <c r="P58">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q58">
+      <c r="Q58" s="2">
         <v>486.43123327236179</v>
       </c>
       <c r="R58">
@@ -6796,7 +6820,7 @@
       <c r="T58">
         <v>366.37131447373167</v>
       </c>
-      <c r="U58">
+      <c r="U58" s="2">
         <v>377.01090067416584</v>
       </c>
       <c r="V58">
@@ -6894,7 +6918,7 @@
       <c r="P59">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q59">
+      <c r="Q59" s="2">
         <v>423.31009234113083</v>
       </c>
       <c r="R59">
@@ -6906,7 +6930,7 @@
       <c r="T59">
         <v>319.70263982251583</v>
       </c>
-      <c r="U59">
+      <c r="U59" s="2">
         <v>328.87564925481502</v>
       </c>
       <c r="V59">
@@ -7004,7 +7028,7 @@
       <c r="P60">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q60">
+      <c r="Q60" s="2">
         <v>504.56422983224405</v>
       </c>
       <c r="R60">
@@ -7016,7 +7040,7 @@
       <c r="T60">
         <v>381.24666633522048</v>
       </c>
-      <c r="U60">
+      <c r="U60" s="2">
         <v>392.52155930597326</v>
       </c>
       <c r="V60">
@@ -7114,7 +7138,7 @@
       <c r="P61">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q61">
+      <c r="Q61" s="2">
         <v>299.44965850444191</v>
       </c>
       <c r="R61">
@@ -7126,7 +7150,7 @@
       <c r="T61">
         <v>240.09006559558469</v>
       </c>
-      <c r="U61">
+      <c r="U61" s="2">
         <v>245.40886832889987</v>
       </c>
       <c r="V61">
@@ -7224,7 +7248,7 @@
       <c r="P62">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q62">
+      <c r="Q62" s="2">
         <v>492.52152196906587</v>
       </c>
       <c r="R62">
@@ -7236,7 +7260,7 @@
       <c r="T62">
         <v>371.51034943020727</v>
       </c>
-      <c r="U62">
+      <c r="U62" s="2">
         <v>382.58071593283046</v>
       </c>
       <c r="V62">
@@ -7334,7 +7358,7 @@
       <c r="P63">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q63">
+      <c r="Q63" s="2">
         <v>331.61218744064723</v>
       </c>
       <c r="R63">
@@ -7346,7 +7370,7 @@
       <c r="T63">
         <v>252.58166540717443</v>
       </c>
-      <c r="U63">
+      <c r="U63" s="2">
         <v>259.787986342473</v>
       </c>
       <c r="V63">
@@ -7444,7 +7468,7 @@
       <c r="P64">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q64">
+      <c r="Q64" s="2">
         <v>447.34693849678774</v>
       </c>
       <c r="R64">
@@ -7456,7 +7480,7 @@
       <c r="T64">
         <v>343.78174585695911</v>
       </c>
-      <c r="U64">
+      <c r="U64" s="2">
         <v>353.51797808966796</v>
       </c>
       <c r="V64">
@@ -7554,7 +7578,7 @@
       <c r="P65">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q65">
+      <c r="Q65" s="2">
         <v>334.62483495366149</v>
       </c>
       <c r="R65">
@@ -7566,7 +7590,7 @@
       <c r="T65">
         <v>275.1114573266276</v>
       </c>
-      <c r="U65">
+      <c r="U65" s="2">
         <v>280.58061079227758</v>
       </c>
       <c r="V65">
@@ -7664,7 +7688,7 @@
       <c r="P66">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q66">
+      <c r="Q66" s="2">
         <v>227.73527407321825</v>
       </c>
       <c r="R66">
@@ -7676,7 +7700,7 @@
       <c r="T66">
         <v>191.74316478611155</v>
       </c>
-      <c r="U66">
+      <c r="U66" s="2">
         <v>194.05861397044026</v>
       </c>
       <c r="V66">
@@ -7774,7 +7798,7 @@
       <c r="P67">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q67">
+      <c r="Q67" s="2">
         <v>256.54172125714348</v>
       </c>
       <c r="R67">
@@ -7786,7 +7810,7 @@
       <c r="T67">
         <v>202.52862204121362</v>
       </c>
-      <c r="U67">
+      <c r="U67" s="2">
         <v>206.09432949987354</v>
       </c>
       <c r="V67">
@@ -7884,7 +7908,7 @@
       <c r="P68">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q68">
+      <c r="Q68" s="2">
         <v>333.3204431953468</v>
       </c>
       <c r="R68">
@@ -7896,7 +7920,7 @@
       <c r="T68">
         <v>271.47961174654421</v>
       </c>
-      <c r="U68">
+      <c r="U68" s="2">
         <v>275.61223785158739</v>
       </c>
       <c r="V68">
@@ -7994,7 +8018,7 @@
       <c r="P69">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q69">
+      <c r="Q69" s="2">
         <v>181.1320196010341</v>
       </c>
       <c r="R69">
@@ -8006,7 +8030,7 @@
       <c r="T69">
         <v>190.28431042805019</v>
       </c>
-      <c r="U69">
+      <c r="U69" s="2">
         <v>189.73235380542491</v>
       </c>
       <c r="V69">
@@ -8104,7 +8128,7 @@
       <c r="P70">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q70">
+      <c r="Q70" s="2">
         <v>475.15152705092032</v>
       </c>
       <c r="R70">
@@ -8116,7 +8140,7 @@
       <c r="T70">
         <v>368.83709605350873</v>
       </c>
-      <c r="U70">
+      <c r="U70" s="2">
         <v>376.26239528573416</v>
       </c>
       <c r="V70">
@@ -8214,7 +8238,7 @@
       <c r="P71">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q71">
+      <c r="Q71" s="2">
         <v>385.28258795859682</v>
       </c>
       <c r="R71">
@@ -8226,7 +8250,7 @@
       <c r="T71">
         <v>307.87400763211059</v>
       </c>
-      <c r="U71">
+      <c r="U71" s="2">
         <v>313.2195339632741</v>
       </c>
       <c r="V71">
@@ -8324,7 +8348,7 @@
       <c r="P72">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q72">
+      <c r="Q72" s="2">
         <v>329.79933546307831</v>
       </c>
       <c r="R72">
@@ -8336,7 +8360,7 @@
       <c r="T72">
         <v>272.15643986205725</v>
       </c>
-      <c r="U72">
+      <c r="U72" s="2">
         <v>276.19062179823464</v>
       </c>
       <c r="V72">
@@ -8434,7 +8458,7 @@
       <c r="P73">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q73">
+      <c r="Q73" s="2">
         <v>570.83603657835158</v>
       </c>
       <c r="R73">
@@ -8446,7 +8470,7 @@
       <c r="T73">
         <v>407.13473700641913</v>
       </c>
-      <c r="U73">
+      <c r="U73" s="2">
         <v>419.25043284477863</v>
       </c>
       <c r="V73">
@@ -8544,7 +8568,7 @@
       <c r="P74">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q74">
+      <c r="Q74" s="2">
         <v>398.84823568275482</v>
       </c>
       <c r="R74">
@@ -8556,7 +8580,7 @@
       <c r="T74">
         <v>328.2306364662889</v>
       </c>
-      <c r="U74">
+      <c r="U74" s="2">
         <v>337.20359452591714</v>
       </c>
       <c r="V74">
@@ -8654,7 +8678,7 @@
       <c r="P75">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q75">
+      <c r="Q75" s="2">
         <v>482.9884185228525</v>
       </c>
       <c r="R75">
@@ -8666,7 +8690,7 @@
       <c r="T75">
         <v>392.21230897239258</v>
       </c>
-      <c r="U75">
+      <c r="U75" s="2">
         <v>403.78775903246054</v>
       </c>
       <c r="V75">
@@ -8764,7 +8788,7 @@
       <c r="P76">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q76">
+      <c r="Q76" s="2">
         <v>340.39458740972657</v>
       </c>
       <c r="R76">
@@ -8776,7 +8800,7 @@
       <c r="T76">
         <v>289.03604302058596</v>
       </c>
-      <c r="U76">
+      <c r="U76" s="2">
         <v>297.05812755854276</v>
       </c>
       <c r="V76">
@@ -8874,7 +8898,7 @@
       <c r="P77">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q77">
+      <c r="Q77" s="2">
         <v>325.6862182067195</v>
       </c>
       <c r="R77">
@@ -8886,7 +8910,7 @@
       <c r="T77">
         <v>276.93554443467417</v>
       </c>
-      <c r="U77">
+      <c r="U77" s="2">
         <v>284.54793663743601</v>
       </c>
       <c r="V77">
@@ -8984,7 +9008,7 @@
       <c r="P78">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q78">
+      <c r="Q78" s="2">
         <v>413.78591235475102</v>
       </c>
       <c r="R78">
@@ -8996,7 +9020,7 @@
       <c r="T78">
         <v>333.01001619703351</v>
       </c>
-      <c r="U78">
+      <c r="U78" s="2">
         <v>341.34925543964602</v>
       </c>
       <c r="V78">
@@ -9094,7 +9118,7 @@
       <c r="P79">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q79">
+      <c r="Q79" s="2">
         <v>515.17221195579657</v>
       </c>
       <c r="R79">
@@ -9106,7 +9130,7 @@
       <c r="T79">
         <v>403.42335920639266</v>
       </c>
-      <c r="U79">
+      <c r="U79" s="2">
         <v>415.05919976143326</v>
       </c>
       <c r="V79">
@@ -9204,7 +9228,7 @@
       <c r="P80">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q80">
+      <c r="Q80" s="2">
         <v>365.01157085829226</v>
       </c>
       <c r="R80">
@@ -9216,7 +9240,7 @@
       <c r="T80">
         <v>285.76728767508115</v>
       </c>
-      <c r="U80">
+      <c r="U80" s="2">
         <v>292.08924415253318</v>
       </c>
       <c r="V80">
@@ -9314,7 +9338,7 @@
       <c r="P81">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q81">
+      <c r="Q81" s="2">
         <v>421.28297120160124</v>
       </c>
       <c r="R81">
@@ -9326,7 +9350,7 @@
       <c r="T81">
         <v>314.04700594598756</v>
       </c>
-      <c r="U81">
+      <c r="U81" s="2">
         <v>322.75549860651853</v>
       </c>
       <c r="V81">
@@ -9424,7 +9448,7 @@
       <c r="P82">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q82">
+      <c r="Q82" s="2">
         <v>400.7626559915704</v>
       </c>
       <c r="R82">
@@ -9436,7 +9460,7 @@
       <c r="T82">
         <v>334.26733995102182</v>
       </c>
-      <c r="U82">
+      <c r="U82" s="2">
         <v>342.29949916483429</v>
       </c>
       <c r="V82">
@@ -9534,7 +9558,7 @@
       <c r="P83">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q83">
+      <c r="Q83" s="2">
         <v>361.20526478631632</v>
       </c>
       <c r="R83">
@@ -9546,7 +9570,7 @@
       <c r="T83">
         <v>299.13826396656043</v>
       </c>
-      <c r="U83">
+      <c r="U83" s="2">
         <v>306.65063358200433</v>
       </c>
       <c r="V83">
@@ -9644,7 +9668,7 @@
       <c r="P84">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q84">
+      <c r="Q84" s="2">
         <v>466.35560001161383</v>
       </c>
       <c r="R84">
@@ -9656,7 +9680,7 @@
       <c r="T84">
         <v>367.24507207161639</v>
       </c>
-      <c r="U84">
+      <c r="U84" s="2">
         <v>377.95673627841398</v>
       </c>
       <c r="V84">
@@ -9754,7 +9778,7 @@
       <c r="P85">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q85">
+      <c r="Q85" s="2">
         <v>355.41347261118449</v>
       </c>
       <c r="R85">
@@ -9766,7 +9790,7 @@
       <c r="T85">
         <v>284.93889835062083</v>
       </c>
-      <c r="U85">
+      <c r="U85" s="2">
         <v>292.51435966375027</v>
       </c>
       <c r="V85">
@@ -9864,7 +9888,7 @@
       <c r="P86">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q86">
+      <c r="Q86" s="2">
         <v>371.43504950282096</v>
       </c>
       <c r="R86">
@@ -9876,7 +9900,7 @@
       <c r="T86">
         <v>302.59249515240919</v>
       </c>
-      <c r="U86">
+      <c r="U86" s="2">
         <v>310.96343330967608</v>
       </c>
       <c r="V86">
@@ -9974,7 +9998,7 @@
       <c r="P87">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q87">
+      <c r="Q87" s="2">
         <v>302.83594841745889</v>
       </c>
       <c r="R87">
@@ -9986,7 +10010,7 @@
       <c r="T87">
         <v>257.45285693934437</v>
       </c>
-      <c r="U87">
+      <c r="U87" s="2">
         <v>262.90491816893388</v>
       </c>
       <c r="V87">
@@ -10084,7 +10108,7 @@
       <c r="P88">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q88">
+      <c r="Q88" s="2">
         <v>422.31391448030712</v>
       </c>
       <c r="R88">
@@ -10096,7 +10120,7 @@
       <c r="T88">
         <v>345.76376753529036</v>
       </c>
-      <c r="U88">
+      <c r="U88" s="2">
         <v>355.05897121514016</v>
       </c>
       <c r="V88">
@@ -10194,7 +10218,7 @@
       <c r="P89">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q89">
+      <c r="Q89" s="2">
         <v>474.649732474882</v>
       </c>
       <c r="R89">
@@ -10206,7 +10230,7 @@
       <c r="T89">
         <v>381.8188031336577</v>
       </c>
-      <c r="U89">
+      <c r="U89" s="2">
         <v>393.14611243479675</v>
       </c>
       <c r="V89">
@@ -10304,7 +10328,7 @@
       <c r="P90">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q90">
+      <c r="Q90" s="2">
         <v>473.34249269899868</v>
       </c>
       <c r="R90">
@@ -10316,7 +10340,7 @@
       <c r="T90">
         <v>418.65707447746496</v>
       </c>
-      <c r="U90">
+      <c r="U90" s="2">
         <v>429.00662693622917</v>
       </c>
       <c r="V90">
@@ -10414,7 +10438,7 @@
       <c r="P91">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q91">
+      <c r="Q91" s="2">
         <v>285.04078085734142</v>
       </c>
       <c r="R91">
@@ -10426,7 +10450,7 @@
       <c r="T91">
         <v>256.47523965841123</v>
       </c>
-      <c r="U91">
+      <c r="U91" s="2">
         <v>261.86482005383704</v>
       </c>
       <c r="V91">
@@ -10524,7 +10548,7 @@
       <c r="P92">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q92">
+      <c r="Q92" s="2">
         <v>398.42045787061102</v>
       </c>
       <c r="R92">
@@ -10536,7 +10560,7 @@
       <c r="T92">
         <v>344.29032371180728</v>
       </c>
-      <c r="U92">
+      <c r="U92" s="2">
         <v>353.25317979646121</v>
       </c>
       <c r="V92">
@@ -10634,7 +10658,7 @@
       <c r="P93">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q93">
+      <c r="Q93" s="2">
         <v>388.14270213191139</v>
       </c>
       <c r="R93">
@@ -10646,7 +10670,7 @@
       <c r="T93">
         <v>330.22093658633497</v>
       </c>
-      <c r="U93">
+      <c r="U93" s="2">
         <v>339.84225843268302</v>
       </c>
       <c r="V93">
@@ -10744,7 +10768,7 @@
       <c r="P94">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q94">
+      <c r="Q94" s="2">
         <v>549.46713343322801</v>
       </c>
       <c r="R94">
@@ -10756,7 +10780,7 @@
       <c r="T94">
         <v>370.03026609607434</v>
       </c>
-      <c r="U94">
+      <c r="U94" s="2">
         <v>380.850129580604</v>
       </c>
       <c r="V94">
@@ -10854,7 +10878,7 @@
       <c r="P95">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q95">
+      <c r="Q95" s="2">
         <v>382.79816288728966</v>
       </c>
       <c r="R95">
@@ -10866,7 +10890,7 @@
       <c r="T95">
         <v>258.93122051684179</v>
       </c>
-      <c r="U95">
+      <c r="U95" s="2">
         <v>266.38670683104908</v>
       </c>
       <c r="V95">
@@ -10964,7 +10988,7 @@
       <c r="P96">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q96">
+      <c r="Q96" s="2">
         <v>433.74749618285159</v>
       </c>
       <c r="R96">
@@ -10976,7 +11000,7 @@
       <c r="T96">
         <v>307.18210794170642</v>
       </c>
-      <c r="U96">
+      <c r="U96" s="2">
         <v>315.50617836472861</v>
       </c>
       <c r="V96">
@@ -11074,7 +11098,7 @@
       <c r="P97">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q97">
+      <c r="Q97" s="2">
         <v>415.08381222967625</v>
       </c>
       <c r="R97">
@@ -11086,7 +11110,7 @@
       <c r="T97">
         <v>290.43864640736444</v>
       </c>
-      <c r="U97">
+      <c r="U97" s="2">
         <v>298.67572523204183</v>
       </c>
       <c r="V97">
@@ -11184,7 +11208,7 @@
       <c r="P98">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q98">
+      <c r="Q98" s="2">
         <v>353.61782448405484</v>
       </c>
       <c r="R98">
@@ -11196,7 +11220,7 @@
       <c r="T98">
         <v>329.49669439569215</v>
       </c>
-      <c r="U98">
+      <c r="U98" s="2">
         <v>339.12822630734348</v>
       </c>
       <c r="V98">
@@ -11294,7 +11318,7 @@
       <c r="P99">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q99">
+      <c r="Q99" s="2">
         <v>270.2031265821085</v>
       </c>
       <c r="R99">
@@ -11306,7 +11330,7 @@
       <c r="T99">
         <v>253.16473170020274</v>
       </c>
-      <c r="U99">
+      <c r="U99" s="2">
         <v>259.97025350244184</v>
       </c>
       <c r="V99">
@@ -11404,7 +11428,7 @@
       <c r="P100">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q100">
+      <c r="Q100" s="2">
         <v>351.73825677566037</v>
       </c>
       <c r="R100">
@@ -11416,7 +11440,7 @@
       <c r="T100">
         <v>313.89922763895379</v>
       </c>
-      <c r="U100">
+      <c r="U100" s="2">
         <v>323.11398119005702</v>
       </c>
       <c r="V100">
@@ -11514,7 +11538,7 @@
       <c r="P101">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q101">
+      <c r="Q101" s="2">
         <v>344.29944568160812</v>
       </c>
       <c r="R101">
@@ -11526,7 +11550,7 @@
       <c r="T101">
         <v>308.95013729423988</v>
       </c>
-      <c r="U101">
+      <c r="U101" s="2">
         <v>317.55405083012738</v>
       </c>
       <c r="V101">
@@ -11576,6 +11600,30 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="Q1:Q1048576">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U1:U1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
NIH kjørt ny stiff etter discards
</commit_message>
<xml_diff>
--- a/data_output/output for F24 stiff 2018-01-18 youngs modulus/all_stiff_output_20180118_1237 GM.xlsx
+++ b/data_output/output for F24 stiff 2018-01-18 youngs modulus/all_stiff_output_20180118_1237 GM.xlsx
@@ -153,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,8 +168,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -181,8 +189,14 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -190,16 +204,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="11" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -483,7 +529,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:XFD69"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="5.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -5667,113 +5715,113 @@
         <v>0.84189000000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A48">
+    <row r="48" spans="1:36" s="4" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
         <v>15</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D48" t="s">
+      <c r="D48" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="4">
         <v>5.6538986599999994E-2</v>
       </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
+      <c r="F48" s="4">
+        <v>0</v>
+      </c>
+      <c r="G48" s="4">
         <v>13.756254169621448</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="4">
         <v>21.306827128907774</v>
       </c>
-      <c r="I48">
-        <v>0</v>
-      </c>
-      <c r="J48">
+      <c r="I48" s="4">
+        <v>0</v>
+      </c>
+      <c r="J48" s="4">
         <v>0.96889704537661503</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="4">
         <v>3900</v>
       </c>
-      <c r="L48">
+      <c r="L48" s="4">
         <v>4356.06841518893</v>
       </c>
-      <c r="M48">
+      <c r="M48" s="4">
         <v>4350</v>
       </c>
-      <c r="N48">
+      <c r="N48" s="4">
         <v>4939.7426844079837</v>
       </c>
-      <c r="O48">
+      <c r="O48" s="4">
         <v>1800</v>
       </c>
-      <c r="P48">
+      <c r="P48" s="4">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q48" s="2">
+      <c r="Q48" s="7">
         <v>439.31224059849467</v>
       </c>
-      <c r="R48">
+      <c r="R48" s="4">
         <v>451.86358727428529</v>
       </c>
-      <c r="S48">
+      <c r="S48" s="4">
         <v>298.8644097839553</v>
       </c>
-      <c r="T48">
+      <c r="T48" s="4">
         <v>307.37902748960164</v>
       </c>
-      <c r="U48" s="2">
+      <c r="U48" s="5">
         <v>316.51229893776127</v>
       </c>
-      <c r="V48">
+      <c r="V48" s="4">
         <v>325.53484750930932</v>
       </c>
-      <c r="W48">
+      <c r="W48" s="4">
         <v>15.295633566128483</v>
       </c>
-      <c r="X48">
+      <c r="X48" s="4">
         <v>16.069037330470405</v>
       </c>
-      <c r="Y48">
+      <c r="Y48" s="4">
         <v>11.337124796907911</v>
       </c>
-      <c r="Z48">
+      <c r="Z48" s="4">
         <v>12.018094711515843</v>
       </c>
-      <c r="AA48">
+      <c r="AA48" s="4">
         <v>213.75666666666601</v>
       </c>
-      <c r="AB48">
+      <c r="AB48" s="4">
         <v>7.1556287832559757</v>
       </c>
-      <c r="AC48">
+      <c r="AC48" s="4">
         <v>7.5174438210755783</v>
       </c>
-      <c r="AD48">
+      <c r="AD48" s="4">
         <v>5.3037526144562888</v>
       </c>
-      <c r="AE48">
+      <c r="AE48" s="4">
         <v>5.6223250946633465</v>
       </c>
-      <c r="AF48" s="1">
+      <c r="AF48" s="6">
         <v>2193939667.7007489</v>
       </c>
-      <c r="AG48" s="1">
+      <c r="AG48" s="6">
         <v>1969253985.9349391</v>
       </c>
-      <c r="AH48" s="1">
+      <c r="AH48" s="6">
         <v>618994449.97484696</v>
       </c>
-      <c r="AI48" s="1">
+      <c r="AI48" s="6">
         <v>906076056.1551491</v>
       </c>
-      <c r="AJ48">
+      <c r="AJ48" s="4">
         <v>0.67510999999999999</v>
       </c>
     </row>
@@ -5826,7 +5874,7 @@
       <c r="P49">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q49" s="2">
+      <c r="Q49" s="8">
         <v>541.07189803289521</v>
       </c>
       <c r="R49">
@@ -7639,443 +7687,443 @@
         <v>0.51300000000000001</v>
       </c>
     </row>
-    <row r="66" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A66">
+    <row r="66" spans="1:36" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="9">
         <v>21</v>
       </c>
-      <c r="B66" t="s">
+      <c r="B66" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D66" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E66">
+      <c r="E66" s="9">
         <v>5.6813447699999998E-2</v>
       </c>
-      <c r="F66">
-        <v>0</v>
-      </c>
-      <c r="G66">
+      <c r="F66" s="9">
+        <v>0</v>
+      </c>
+      <c r="G66" s="9">
         <v>2.1036006397688389</v>
       </c>
-      <c r="H66">
+      <c r="H66" s="9">
         <v>149.60184681921905</v>
       </c>
-      <c r="I66">
-        <v>0</v>
-      </c>
-      <c r="J66">
+      <c r="I66" s="9">
+        <v>0</v>
+      </c>
+      <c r="J66" s="9">
         <v>0.98658780955120451</v>
       </c>
-      <c r="K66">
+      <c r="K66" s="9">
         <v>3900</v>
       </c>
-      <c r="L66">
+      <c r="L66" s="9">
         <v>4460.3650172829348</v>
       </c>
-      <c r="M66">
+      <c r="M66" s="9">
         <v>4300</v>
       </c>
-      <c r="N66">
+      <c r="N66" s="9">
         <v>4844.9820125184569</v>
       </c>
-      <c r="O66">
+      <c r="O66" s="9">
         <v>1800</v>
       </c>
-      <c r="P66">
+      <c r="P66" s="9">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q66" s="2">
+      <c r="Q66" s="10">
         <v>227.73527407321825</v>
       </c>
-      <c r="R66">
+      <c r="R66" s="9">
         <v>231.39469236662129</v>
       </c>
-      <c r="S66">
+      <c r="S66" s="9">
         <v>189.72641489424672</v>
       </c>
-      <c r="T66">
+      <c r="T66" s="9">
         <v>191.74316478611155</v>
       </c>
-      <c r="U66" s="2">
+      <c r="U66" s="10">
         <v>194.05861397044026</v>
       </c>
-      <c r="V66">
+      <c r="V66" s="9">
         <v>196.27297868352156</v>
       </c>
-      <c r="W66">
+      <c r="W66" s="9">
         <v>20.955350024266927</v>
       </c>
-      <c r="X66">
+      <c r="X66" s="9">
         <v>22.582424491800538</v>
       </c>
-      <c r="Y66">
+      <c r="Y66" s="9">
         <v>10.141895411270632</v>
       </c>
-      <c r="Z66">
+      <c r="Z66" s="9">
         <v>11.020717312378595</v>
       </c>
-      <c r="AA66">
+      <c r="AA66" s="9">
         <v>190.22666666666601</v>
       </c>
-      <c r="AB66">
+      <c r="AB66" s="9">
         <v>11.015989709259305</v>
       </c>
-      <c r="AC66">
+      <c r="AC66" s="9">
         <v>11.871324293019178</v>
       </c>
-      <c r="AD66">
+      <c r="AD66" s="9">
         <v>5.3314793288378777</v>
       </c>
-      <c r="AE66">
+      <c r="AE66" s="9">
         <v>5.7934660294974245</v>
       </c>
-      <c r="AF66" s="1">
+      <c r="AF66" s="11">
         <v>610300822.92235446</v>
       </c>
-      <c r="AG66" s="1">
+      <c r="AG66" s="11">
         <v>697741720.42220545</v>
       </c>
-      <c r="AH66" s="1">
+      <c r="AH66" s="11">
         <v>1058787161.2883569</v>
       </c>
-      <c r="AI66" s="1">
+      <c r="AI66" s="11">
         <v>910571405.76829791</v>
       </c>
-      <c r="AJ66">
+      <c r="AJ66" s="9">
         <v>0.58221999999999996</v>
       </c>
     </row>
-    <row r="67" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A67">
+    <row r="67" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="12">
         <v>21</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B67" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="C67" t="s">
+      <c r="C67" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D67" t="s">
+      <c r="D67" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E67">
+      <c r="E67" s="12">
         <v>5.6813447699999998E-2</v>
       </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67">
+      <c r="F67" s="12">
+        <v>0</v>
+      </c>
+      <c r="G67" s="12">
         <v>3.4579030327654814</v>
       </c>
-      <c r="H67">
+      <c r="H67" s="12">
         <v>131.81513915940909</v>
       </c>
-      <c r="I67">
-        <v>0</v>
-      </c>
-      <c r="J67">
+      <c r="I67" s="12">
+        <v>0</v>
+      </c>
+      <c r="J67" s="12">
         <v>0.99733730006338173</v>
       </c>
-      <c r="K67">
+      <c r="K67" s="12">
         <v>3900</v>
       </c>
-      <c r="L67">
+      <c r="L67" s="12">
         <v>4375.5452387152081</v>
       </c>
-      <c r="M67">
+      <c r="M67" s="12">
         <v>4200</v>
       </c>
-      <c r="N67">
+      <c r="N67" s="12">
         <v>4410.0008685965558</v>
       </c>
-      <c r="O67">
+      <c r="O67" s="12">
         <v>1800</v>
       </c>
-      <c r="P67">
+      <c r="P67" s="12">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q67" s="2">
+      <c r="Q67" s="13">
         <v>256.54172125714348</v>
       </c>
-      <c r="R67">
+      <c r="R67" s="12">
         <v>261.90616751374029</v>
       </c>
-      <c r="S67">
+      <c r="S67" s="12">
         <v>199.35759705595697</v>
       </c>
-      <c r="T67">
+      <c r="T67" s="12">
         <v>202.52862204121362</v>
       </c>
-      <c r="U67" s="2">
+      <c r="U67" s="13">
         <v>206.09432949987354</v>
       </c>
-      <c r="V67">
+      <c r="V67" s="12">
         <v>209.53921762186727</v>
       </c>
-      <c r="W67">
+      <c r="W67" s="12">
         <v>19.72241128077323</v>
       </c>
-      <c r="X67">
+      <c r="X67" s="12">
         <v>20.274797985329673</v>
       </c>
-      <c r="Y67">
+      <c r="Y67" s="12">
         <v>10.711349544959262</v>
       </c>
-      <c r="Z67">
+      <c r="Z67" s="12">
         <v>11.704736271250484</v>
       </c>
-      <c r="AA67">
+      <c r="AA67" s="12">
         <v>186.446666666666</v>
       </c>
-      <c r="AB67">
+      <c r="AB67" s="12">
         <v>10.578044452805074</v>
       </c>
-      <c r="AC67">
+      <c r="AC67" s="12">
         <v>10.874315077768305</v>
       </c>
-      <c r="AD67">
+      <c r="AD67" s="12">
         <v>5.7449938561300637</v>
       </c>
-      <c r="AE67">
+      <c r="AE67" s="12">
         <v>6.277793258796363</v>
       </c>
-      <c r="AF67" s="1">
+      <c r="AF67" s="14">
         <v>750918293.09424496</v>
       </c>
-      <c r="AG67" s="1">
+      <c r="AG67" s="14">
         <v>976010589.08817828</v>
       </c>
-      <c r="AH67" s="1">
+      <c r="AH67" s="14">
         <v>646916059.24494886</v>
       </c>
-      <c r="AI67" s="1">
+      <c r="AI67" s="14">
         <v>756770854.79605603</v>
       </c>
-      <c r="AJ67">
+      <c r="AJ67" s="12">
         <v>0.60899999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A68">
+    <row r="68" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="12">
         <v>21</v>
       </c>
-      <c r="B68" t="s">
+      <c r="B68" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="D68" t="s">
+      <c r="D68" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="E68">
+      <c r="E68" s="12">
         <v>5.6813447699999998E-2</v>
       </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
+      <c r="F68" s="12">
+        <v>0</v>
+      </c>
+      <c r="G68" s="12">
         <v>5.3477753889702742</v>
       </c>
-      <c r="H68">
+      <c r="H68" s="12">
         <v>192.7043546363264</v>
       </c>
-      <c r="I68">
-        <v>0</v>
-      </c>
-      <c r="J68">
+      <c r="I68" s="12">
+        <v>0</v>
+      </c>
+      <c r="J68" s="12">
         <v>0.97259762105558334</v>
       </c>
-      <c r="K68">
+      <c r="K68" s="12">
         <v>3850</v>
       </c>
-      <c r="L68">
+      <c r="L68" s="12">
         <v>4666.8948265374402</v>
       </c>
-      <c r="M68">
+      <c r="M68" s="12">
         <v>4650</v>
       </c>
-      <c r="N68">
+      <c r="N68" s="12">
         <v>4866.0009022209788</v>
       </c>
-      <c r="O68">
+      <c r="O68" s="12">
         <v>1800</v>
       </c>
-      <c r="P68">
+      <c r="P68" s="12">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q68" s="2">
+      <c r="Q68" s="13">
         <v>333.3204431953468</v>
       </c>
-      <c r="R68">
+      <c r="R68" s="12">
         <v>339.61179077846373</v>
       </c>
-      <c r="S68">
+      <c r="S68" s="12">
         <v>267.83742521488307</v>
       </c>
-      <c r="T68">
+      <c r="T68" s="12">
         <v>271.47961174654421</v>
       </c>
-      <c r="U68" s="2">
+      <c r="U68" s="13">
         <v>275.61223785158739</v>
       </c>
-      <c r="V68">
+      <c r="V68" s="12">
         <v>279.58737759793831</v>
       </c>
-      <c r="W68">
+      <c r="W68" s="12">
         <v>15.556906051053582</v>
       </c>
-      <c r="X68">
+      <c r="X68" s="12">
         <v>19.97752673764278</v>
       </c>
-      <c r="Y68">
+      <c r="Y68" s="12">
         <v>7.771519760845452</v>
       </c>
-      <c r="Z68">
+      <c r="Z68" s="12">
         <v>8.2686685835398723</v>
       </c>
-      <c r="AA68">
+      <c r="AA68" s="12">
         <v>185.23333333333301</v>
       </c>
-      <c r="AB68">
+      <c r="AB68" s="12">
         <v>8.3985456457010663</v>
       </c>
-      <c r="AC68">
+      <c r="AC68" s="12">
         <v>10.785060322643233</v>
       </c>
-      <c r="AD68">
+      <c r="AD68" s="12">
         <v>4.1955298330999451</v>
       </c>
-      <c r="AE68">
+      <c r="AE68" s="12">
         <v>4.4639204158034307</v>
       </c>
-      <c r="AF68" s="1">
+      <c r="AF68" s="14">
         <v>561500008.77113318</v>
       </c>
-      <c r="AG68" s="1">
+      <c r="AG68" s="14">
         <v>546872301.90524626</v>
       </c>
-      <c r="AH68" s="1">
+      <c r="AH68" s="14">
         <v>997350324.77485025</v>
       </c>
-      <c r="AI68" s="1">
+      <c r="AI68" s="14">
         <v>1369057422.7725739</v>
       </c>
-      <c r="AJ68">
+      <c r="AJ68" s="12">
         <v>0.60467000000000004</v>
       </c>
     </row>
-    <row r="69" spans="1:36" x14ac:dyDescent="0.3">
-      <c r="A69">
+    <row r="69" spans="1:36" s="15" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="15">
         <v>21</v>
       </c>
-      <c r="B69" t="s">
+      <c r="B69" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D69" t="s">
+      <c r="D69" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="E69">
+      <c r="E69" s="15">
         <v>5.6813447699999998E-2</v>
       </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-      <c r="G69">
+      <c r="F69" s="15">
+        <v>0</v>
+      </c>
+      <c r="G69" s="15">
         <v>-0.48365985988399812</v>
       </c>
-      <c r="H69">
+      <c r="H69" s="15">
         <v>198.78772990489287</v>
       </c>
-      <c r="I69">
-        <v>0</v>
-      </c>
-      <c r="J69">
+      <c r="I69" s="15">
+        <v>0</v>
+      </c>
+      <c r="J69" s="15">
         <v>0.96560891775036861</v>
       </c>
-      <c r="K69">
+      <c r="K69" s="15">
         <v>3850</v>
       </c>
-      <c r="L69">
+      <c r="L69" s="15">
         <v>4280.4608591303295</v>
       </c>
-      <c r="M69">
+      <c r="M69" s="15">
         <v>4250</v>
       </c>
-      <c r="N69">
+      <c r="N69" s="15">
         <v>4966.798800048623</v>
       </c>
-      <c r="O69">
+      <c r="O69" s="15">
         <v>1800</v>
       </c>
-      <c r="P69">
+      <c r="P69" s="15">
         <v>2019.9772466778345</v>
       </c>
-      <c r="Q69" s="2">
+      <c r="Q69" s="16">
         <v>181.1320196010341</v>
       </c>
-      <c r="R69">
+      <c r="R69" s="15">
         <v>180.10982465171188</v>
       </c>
-      <c r="S69">
+      <c r="S69" s="15">
         <v>190.73964549956119</v>
       </c>
-      <c r="T69">
+      <c r="T69" s="15">
         <v>190.28431042805019</v>
       </c>
-      <c r="U69" s="2">
+      <c r="U69" s="16">
         <v>189.73235380542491</v>
       </c>
-      <c r="V69">
+      <c r="V69" s="15">
         <v>189.21882492093368</v>
       </c>
-      <c r="W69">
+      <c r="W69" s="15">
         <v>21.352346180776209</v>
       </c>
-      <c r="X69">
+      <c r="X69" s="15">
         <v>23.278144187382996</v>
       </c>
-      <c r="Y69">
+      <c r="Y69" s="15">
         <v>8.9547924078248027</v>
       </c>
-      <c r="Z69">
+      <c r="Z69" s="15">
         <v>9.7099007384635776</v>
       </c>
-      <c r="AA69">
+      <c r="AA69" s="15">
         <v>179.43666666666601</v>
       </c>
-      <c r="AB69">
+      <c r="AB69" s="15">
         <v>11.89965606106683</v>
       </c>
-      <c r="AC69">
+      <c r="AC69" s="15">
         <v>12.972902707018118</v>
       </c>
-      <c r="AD69">
+      <c r="AD69" s="15">
         <v>4.9905030973740976</v>
       </c>
-      <c r="AE69">
+      <c r="AE69" s="15">
         <v>5.4113247413926615</v>
       </c>
-      <c r="AF69" s="1">
+      <c r="AF69" s="17">
         <v>344019711.25508064</v>
       </c>
-      <c r="AG69" s="1">
+      <c r="AG69" s="17">
         <v>426145542.0037145</v>
       </c>
-      <c r="AH69" s="1">
+      <c r="AH69" s="17">
         <v>903694067.54494667</v>
       </c>
-      <c r="AI69" s="1">
+      <c r="AI69" s="17">
         <v>876568736.04662704</v>
       </c>
-      <c r="AJ69">
+      <c r="AJ69" s="15">
         <v>0.68110999999999999</v>
       </c>
     </row>
@@ -11625,5 +11673,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>